<commit_message>
Added BOM assembly count information to BOM Excel file.
</commit_message>
<xml_diff>
--- a/Kicad-Faraday/OutputFiles/Faraday-REVC(BOM).xlsx
+++ b/Kicad-Faraday/OutputFiles/Faraday-REVC(BOM).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="263">
   <si>
     <t>PTS645SM43SMTR92_LFS</t>
   </si>
@@ -796,6 +796,18 @@
   </si>
   <si>
     <t>Revision C</t>
+  </si>
+  <si>
+    <t>Assembly Line Items</t>
+  </si>
+  <si>
+    <t>Placement Count</t>
+  </si>
+  <si>
+    <t>SMT</t>
+  </si>
+  <si>
+    <t>Through-Hole</t>
   </si>
 </sst>
 </file>
@@ -1287,7 +1299,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1324,6 +1336,21 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="26" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" xfId="34" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" xfId="34" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="27" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1680,25 +1707,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.59765625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10" t="s">
         <v>257</v>
       </c>
@@ -1716,7 +1743,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>139</v>
       </c>
@@ -1740,7 +1767,7 @@
       </c>
       <c r="H2" s="14"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1762,7 +1789,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1788,7 +1815,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1814,7 +1841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1840,7 +1867,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1866,7 +1893,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1892,7 +1919,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1918,7 +1945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1944,7 +1971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1970,7 +1997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1996,7 +2023,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -2022,7 +2049,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -2048,7 +2075,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -2074,7 +2101,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -2100,7 +2127,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -2126,7 +2153,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -2146,7 +2173,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -2168,7 +2195,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
@@ -2190,7 +2217,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -2209,7 +2236,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -2231,7 +2258,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -2253,7 +2280,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -2275,7 +2302,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -2297,7 +2324,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -2319,7 +2346,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -2341,7 +2368,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>55</v>
       </c>
@@ -2360,7 +2387,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
@@ -2382,7 +2409,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2401,7 +2428,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>249</v>
       </c>
@@ -2420,7 +2447,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -2442,7 +2469,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -2464,7 +2491,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -2486,7 +2513,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -2508,7 +2535,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
@@ -2527,7 +2554,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -2546,7 +2573,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -2565,7 +2592,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -2584,7 +2611,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>79</v>
       </c>
@@ -2606,7 +2633,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
@@ -2628,7 +2655,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>2</v>
       </c>
@@ -2652,7 +2679,7 @@
       </c>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>360</v>
       </c>
@@ -2676,7 +2703,7 @@
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
@@ -2700,7 +2727,7 @@
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
@@ -2724,7 +2751,7 @@
       </c>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>89</v>
       </c>
@@ -2748,7 +2775,7 @@
       </c>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>91</v>
       </c>
@@ -2772,7 +2799,7 @@
       </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>93</v>
       </c>
@@ -2796,7 +2823,7 @@
       </c>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>95</v>
       </c>
@@ -2820,7 +2847,7 @@
       </c>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>36</v>
       </c>
@@ -2839,7 +2866,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>99</v>
       </c>
@@ -2861,7 +2888,7 @@
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
@@ -2883,7 +2910,7 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
@@ -2905,7 +2932,7 @@
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
@@ -2927,7 +2954,7 @@
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>109</v>
       </c>
@@ -2949,7 +2976,7 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>112</v>
       </c>
@@ -2971,7 +2998,7 @@
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>115</v>
       </c>
@@ -2993,7 +3020,7 @@
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>118</v>
       </c>
@@ -3015,7 +3042,7 @@
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>120</v>
       </c>
@@ -3037,7 +3064,7 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>252</v>
       </c>
@@ -3059,7 +3086,7 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>125</v>
       </c>
@@ -3081,7 +3108,7 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>128</v>
       </c>
@@ -3103,7 +3130,7 @@
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>130</v>
       </c>
@@ -3125,7 +3152,7 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>132</v>
       </c>
@@ -3147,7 +3174,7 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>135</v>
       </c>
@@ -3169,7 +3196,7 @@
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>137</v>
       </c>
@@ -3191,7 +3218,7 @@
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>190</v>
       </c>
@@ -3213,7 +3240,7 @@
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>165</v>
       </c>
@@ -3235,9 +3262,47 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E69"/>
-      <c r="F69"/>
+    <row r="69" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="1"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A70" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="E70"/>
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A71" s="18">
+        <f>COUNTA(A3:A68)-COUNTA(A68,A67,A50,A39,A38,A36,A37,A34,A30,A31,A32,A21,A18)</f>
+        <v>53</v>
+      </c>
+      <c r="B71" s="17">
+        <f>SUM(B3:B68)-SUM(B68,B67,B50,B39,B38,B37,B36,B35,B32,B31,B30,B18,B21)</f>
+        <v>118</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B72" s="17">
+        <f>SUM(B35)</f>
+        <v>1</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>262</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>